<commit_message>
fix: forecast graphs and page
</commit_message>
<xml_diff>
--- a/fastapi-backend/freight_yearly 2035.xlsx
+++ b/fastapi-backend/freight_yearly 2035.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Year</t>
   </si>
@@ -36,6 +36,9 @@
   <si>
     <t>95%_upper</t>
   </si>
+  <si>
+    <t>null</t>
+  </si>
 </sst>
 </file>
 
@@ -43,11 +46,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -61,44 +64,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -125,6 +90,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -133,6 +121,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -143,14 +138,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -163,16 +151,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -180,29 +198,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -224,6 +220,60 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -236,31 +286,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -278,7 +310,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -290,6 +346,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -302,25 +364,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -332,79 +382,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -415,36 +411,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -467,6 +433,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -481,6 +462,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -488,6 +484,15 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -506,160 +511,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1016,13 +1012,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
+  <cols>
+    <col min="2" max="7" width="12.625"/>
+  </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="1" t="s">
@@ -1231,223 +1230,236 @@
         <v>1.10438302278</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:1">
       <c r="A25">
-        <v>2025</v>
-      </c>
-      <c r="C25">
-        <v>1.23320543893493</v>
-      </c>
-      <c r="D25">
-        <v>1.16348798342771</v>
-      </c>
-      <c r="E25">
-        <v>1.29867758232444</v>
-      </c>
-      <c r="F25">
-        <v>1.12437328331197</v>
-      </c>
-      <c r="G25">
-        <v>1.33781454899875</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
       <c r="A26">
-        <v>2026</v>
-      </c>
-      <c r="C26">
-        <v>1.28021193843452</v>
-      </c>
-      <c r="D26">
-        <v>1.16882493017821</v>
-      </c>
-      <c r="E26">
-        <v>1.38892003294726</v>
-      </c>
-      <c r="F26">
-        <v>1.11544532966738</v>
-      </c>
-      <c r="G26">
-        <v>1.4426334478736</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27">
-        <v>2027</v>
+        <v>2025</v>
+      </c>
+      <c r="B27" t="s">
+        <v>7</v>
       </c>
       <c r="C27">
-        <v>1.32220042939316</v>
+        <v>1.23320543893493</v>
       </c>
       <c r="D27">
-        <v>1.20111252598971</v>
+        <v>1.16348798342771</v>
       </c>
       <c r="E27">
-        <v>1.43914414973646</v>
+        <v>1.29867758232444</v>
       </c>
       <c r="F27">
-        <v>1.13689058642627</v>
+        <v>1.12437328331197</v>
       </c>
       <c r="G27">
-        <v>1.50384614189235</v>
+        <v>1.33781454899875</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28">
-        <v>2028</v>
+        <v>2026</v>
       </c>
       <c r="C28">
-        <v>1.35777989232209</v>
+        <v>1.28021193843452</v>
       </c>
       <c r="D28">
-        <v>1.22424185034809</v>
+        <v>1.16882493017821</v>
       </c>
       <c r="E28">
-        <v>1.490003457253</v>
+        <v>1.38892003294726</v>
       </c>
       <c r="F28">
-        <v>1.14788550288178</v>
+        <v>1.11544532966738</v>
       </c>
       <c r="G28">
-        <v>1.55423847918459</v>
+        <v>1.4426334478736</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29">
-        <v>2029</v>
+        <v>2027</v>
       </c>
       <c r="C29">
-        <v>1.3945811439168</v>
+        <v>1.32220042939316</v>
       </c>
       <c r="D29">
-        <v>1.2582764095012</v>
+        <v>1.20111252598971</v>
       </c>
       <c r="E29">
-        <v>1.526873814252</v>
+        <v>1.43914414973646</v>
       </c>
       <c r="F29">
-        <v>1.18125483891426</v>
+        <v>1.13689058642627</v>
       </c>
       <c r="G29">
-        <v>1.59497262344389</v>
+        <v>1.50384614189235</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30">
-        <v>2030</v>
+        <v>2028</v>
       </c>
       <c r="C30">
-        <v>1.43015409202864</v>
+        <v>1.35777989232209</v>
       </c>
       <c r="D30">
-        <v>1.29275084029971</v>
+        <v>1.22424185034809</v>
       </c>
       <c r="E30">
-        <v>1.56901644026695</v>
+        <v>1.490003457253</v>
       </c>
       <c r="F30">
-        <v>1.21287666693423</v>
+        <v>1.14788550288178</v>
       </c>
       <c r="G30">
-        <v>1.63782717668923</v>
+        <v>1.55423847918459</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31">
-        <v>2031</v>
+        <v>2029</v>
       </c>
       <c r="C31">
-        <v>1.46241393189524</v>
+        <v>1.3945811439168</v>
       </c>
       <c r="D31">
-        <v>1.32132775367511</v>
+        <v>1.2582764095012</v>
       </c>
       <c r="E31">
-        <v>1.60971159380031</v>
+        <v>1.526873814252</v>
       </c>
       <c r="F31">
-        <v>1.25323345029776</v>
+        <v>1.18125483891426</v>
       </c>
       <c r="G31">
-        <v>1.68626569606279</v>
+        <v>1.59497262344389</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32">
-        <v>2032</v>
+        <v>2030</v>
       </c>
       <c r="C32">
-        <v>1.49649185391322</v>
+        <v>1.43015409202864</v>
       </c>
       <c r="D32">
-        <v>1.34856882622453</v>
+        <v>1.29275084029971</v>
       </c>
       <c r="E32">
-        <v>1.64392583599581</v>
+        <v>1.56901644026695</v>
       </c>
       <c r="F32">
-        <v>1.27261832565878</v>
+        <v>1.21287666693423</v>
       </c>
       <c r="G32">
-        <v>1.71390462598303</v>
+        <v>1.63782717668923</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33">
-        <v>2033</v>
+        <v>2031</v>
       </c>
       <c r="C33">
-        <v>1.52622828746084</v>
+        <v>1.46241393189524</v>
       </c>
       <c r="D33">
-        <v>1.38320132105414</v>
+        <v>1.32132775367511</v>
       </c>
       <c r="E33">
-        <v>1.67771797786909</v>
+        <v>1.60971159380031</v>
       </c>
       <c r="F33">
-        <v>1.29595294218372</v>
+        <v>1.25323345029776</v>
       </c>
       <c r="G33">
-        <v>1.74764320492998</v>
+        <v>1.68626569606279</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34">
-        <v>2034</v>
+        <v>2032</v>
       </c>
       <c r="C34">
-        <v>1.5562985403817</v>
+        <v>1.49649185391322</v>
       </c>
       <c r="D34">
-        <v>1.40883943138125</v>
+        <v>1.34856882622453</v>
       </c>
       <c r="E34">
-        <v>1.70404448653468</v>
+        <v>1.64392583599581</v>
       </c>
       <c r="F34">
-        <v>1.32527886998157</v>
+        <v>1.27261832565878</v>
       </c>
       <c r="G34">
-        <v>1.7941087090515</v>
+        <v>1.71390462598303</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35">
+        <v>2033</v>
+      </c>
+      <c r="C35">
+        <v>1.52622828746084</v>
+      </c>
+      <c r="D35">
+        <v>1.38320132105414</v>
+      </c>
+      <c r="E35">
+        <v>1.67771797786909</v>
+      </c>
+      <c r="F35">
+        <v>1.29595294218372</v>
+      </c>
+      <c r="G35">
+        <v>1.74764320492998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36">
+        <v>2034</v>
+      </c>
+      <c r="C36">
+        <v>1.5562985403817</v>
+      </c>
+      <c r="D36">
+        <v>1.40883943138125</v>
+      </c>
+      <c r="E36">
+        <v>1.70404448653468</v>
+      </c>
+      <c r="F36">
+        <v>1.32527886998157</v>
+      </c>
+      <c r="G36">
+        <v>1.7941087090515</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37">
         <v>2035</v>
       </c>
-      <c r="C35">
+      <c r="C37">
         <v>1.5893208755063</v>
       </c>
-      <c r="D35">
+      <c r="D37">
         <v>1.43665511016774</v>
       </c>
-      <c r="E35">
+      <c r="E37">
         <v>1.74754875187646</v>
       </c>
-      <c r="F35">
+      <c r="F37">
         <v>1.34190072105448</v>
       </c>
-      <c r="G35">
+      <c r="G37">
         <v>1.82174253722935</v>
       </c>
     </row>

</xml_diff>